<commit_message>
Last update - 05/05/2022
</commit_message>
<xml_diff>
--- a/Working Records.xlsx
+++ b/Working Records.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_Files\Working_Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E246F129-2139-4C27-AEFB-380A84B52906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52596C7C-51D1-4F9A-A625-5CD0F79D0B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8583" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8596" uniqueCount="554">
   <si>
     <t>Agent</t>
   </si>
@@ -1696,6 +1696,9 @@
   </si>
   <si>
     <t>Comida Gato</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -1807,13 +1810,45 @@
   </cellStyles>
   <dxfs count="50">
     <dxf>
-      <numFmt numFmtId="9" formatCode="&quot;$&quot;\ #,##0;\-&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2047,7 +2082,13 @@
       <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;\ #,##0;\-&quot;$&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2077,44 +2118,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2166,57 +2169,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Records" displayName="Records" ref="A1:L533" totalsRowCount="1" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:L532" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Records" displayName="Records" ref="A1:L534" totalsRowCount="1" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="A1:L533" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="11">
       <filters>
-        <dateGroupItem year="2022" month="4" dateTimeGrouping="month"/>
+        <dateGroupItem year="2022" month="5" dateTimeGrouping="month"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A514:L532">
-    <sortCondition ref="L1:L532"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A514:L531">
+    <sortCondition ref="L1:L531"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Client" totalsRowLabel="Total" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Institution" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Subject" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Agent" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Payment Method" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Total" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Earnings" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Credit" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Balance" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Client" totalsRowLabel="Total" dataDxfId="47" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="46" totalsRowDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Institution" dataDxfId="45" totalsRowDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Subject" dataDxfId="44" totalsRowDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Agent" dataDxfId="43" totalsRowDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Payment Method" dataDxfId="42" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Total" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Earnings" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Credit" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status" dataDxfId="38" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Balance" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(Records[[#This Row],[Total]]-Records[[#This Row],[Credit]]=0,"—",Records[[#This Row],[Total]]-Records[[#This Row],[Credit]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date" totalsRowFunction="count" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date" totalsRowFunction="count" dataDxfId="36" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C9C4AE10-93E1-4E87-8E3E-DD1F37F42F76}" name="Tabla3" displayName="Tabla3" ref="A1:I996" totalsRowCount="1" headerRowDxfId="23">
-  <autoFilter ref="A1:I995" xr:uid="{C9C4AE10-93E1-4E87-8E3E-DD1F37F42F76}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C9C4AE10-93E1-4E87-8E3E-DD1F37F42F76}" name="Tabla3" displayName="Tabla3" ref="A1:I998" totalsRowCount="1" headerRowDxfId="35">
+  <autoFilter ref="A1:I997" xr:uid="{C9C4AE10-93E1-4E87-8E3E-DD1F37F42F76}">
     <filterColumn colId="6">
       <filters>
         <dateGroupItem year="2022" month="5" dateTimeGrouping="month"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A916:I995">
-    <sortCondition ref="G1:G995"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A916:I997">
+    <sortCondition ref="G1:G997"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{886A6CAF-EB23-4F8B-A9DB-A3696D04F8F6}" name="Description" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{36CBABCB-9F04-4ECE-B9ED-1C62D8F54929}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{7A71AD62-C67C-4184-B2AE-343FDF2E1AAB}" name="Amount" totalsRowFunction="sum" totalsRowDxfId="2" dataCellStyle="Moneda [0]"/>
-    <tableColumn id="4" xr3:uid="{005E1104-EE5B-420E-8EDD-888B113AEB44}" name="Credit" totalsRowFunction="sum" totalsRowDxfId="1" dataCellStyle="Moneda [0]"/>
-    <tableColumn id="5" xr3:uid="{79A76D31-0FB1-4A1E-A4E4-EF68447E9886}" name="Balance" totalsRowFunction="sum" totalsRowDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{7A71AD62-C67C-4184-B2AE-343FDF2E1AAB}" name="Amount" totalsRowFunction="sum" totalsRowDxfId="34" dataCellStyle="Moneda [0]"/>
+    <tableColumn id="4" xr3:uid="{005E1104-EE5B-420E-8EDD-888B113AEB44}" name="Credit" totalsRowFunction="sum" totalsRowDxfId="33" dataCellStyle="Moneda [0]"/>
+    <tableColumn id="5" xr3:uid="{79A76D31-0FB1-4A1E-A4E4-EF68447E9886}" name="Balance" totalsRowFunction="sum" totalsRowDxfId="32"/>
     <tableColumn id="6" xr3:uid="{D362C1AF-0EF8-4D53-A2D0-3D14E390CD47}" name="Status"/>
-    <tableColumn id="7" xr3:uid="{10384694-AE38-4DBA-87F2-E798B0B6DE3A}" name="Date" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{10384694-AE38-4DBA-87F2-E798B0B6DE3A}" name="Date" dataDxfId="31"/>
     <tableColumn id="8" xr3:uid="{D69A3575-5F26-4C6F-B4D3-F11B2434D87D}" name="Month"/>
     <tableColumn id="9" xr3:uid="{1D409F58-BD51-4914-AEE2-CFE94D9A7A13}" name="Year"/>
   </tableColumns>
@@ -2487,11 +2490,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L540"/>
+  <dimension ref="A1:L541"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H529" sqref="H529"/>
+      <selection pane="bottomLeft" activeCell="H539" sqref="H539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22518,7 +22521,7 @@
         <v>44645</v>
       </c>
     </row>
-    <row r="514" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A514" s="1" t="s">
         <v>46</v>
       </c>
@@ -22557,7 +22560,7 @@
         <v>44653</v>
       </c>
     </row>
-    <row r="515" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A515" s="1" t="s">
         <v>46</v>
       </c>
@@ -22596,7 +22599,7 @@
         <v>44653</v>
       </c>
     </row>
-    <row r="516" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A516" s="1" t="s">
         <v>46</v>
       </c>
@@ -22635,7 +22638,7 @@
         <v>44656</v>
       </c>
     </row>
-    <row r="517" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A517" s="1" t="s">
         <v>46</v>
       </c>
@@ -22674,7 +22677,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="518" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A518" s="1" t="s">
         <v>153</v>
       </c>
@@ -22713,7 +22716,7 @@
         <v>44664</v>
       </c>
     </row>
-    <row r="519" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A519" s="1" t="s">
         <v>533</v>
       </c>
@@ -22752,7 +22755,7 @@
         <v>44665</v>
       </c>
     </row>
-    <row r="520" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A520" s="1" t="s">
         <v>46</v>
       </c>
@@ -22791,7 +22794,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="521" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A521" s="1" t="s">
         <v>505</v>
       </c>
@@ -22830,7 +22833,7 @@
         <v>44671</v>
       </c>
     </row>
-    <row r="522" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A522" s="1" t="s">
         <v>535</v>
       </c>
@@ -22869,7 +22872,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="523" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A523" s="1" t="s">
         <v>142</v>
       </c>
@@ -22908,7 +22911,7 @@
         <v>44673</v>
       </c>
     </row>
-    <row r="524" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A524" s="1" t="s">
         <v>356</v>
       </c>
@@ -22947,7 +22950,7 @@
         <v>44674</v>
       </c>
     </row>
-    <row r="525" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A525" s="1" t="s">
         <v>142</v>
       </c>
@@ -22986,7 +22989,7 @@
         <v>44674</v>
       </c>
     </row>
-    <row r="526" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A526" s="1" t="s">
         <v>535</v>
       </c>
@@ -23025,9 +23028,9 @@
         <v>44674</v>
       </c>
     </row>
-    <row r="527" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A527" s="1" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="B527" s="1" t="s">
         <v>5</v>
@@ -23036,7 +23039,7 @@
         <v>10</v>
       </c>
       <c r="D527" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="E527" s="1" t="s">
         <v>13</v>
@@ -23045,37 +23048,37 @@
         <v>14</v>
       </c>
       <c r="G527" s="3">
-        <v>28000</v>
+        <v>30000</v>
       </c>
       <c r="H527" s="3">
-        <v>28000</v>
+        <v>30000</v>
       </c>
       <c r="I527" s="3">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="J527" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="K527" s="3">
-        <f>IF(Records[[#This Row],[Total]]-Records[[#This Row],[Credit]]=0,"—",Records[[#This Row],[Total]]-Records[[#This Row],[Credit]])</f>
-        <v>28000</v>
+      <c r="K527" s="3" t="str">
+        <f>IF(Records[[#This Row],[Total]]-Records[[#This Row],[Credit]]=0,"—",Records[[#This Row],[Total]]-Records[[#This Row],[Credit]])</f>
+        <v>—</v>
       </c>
       <c r="L527" s="2">
         <v>44676</v>
       </c>
     </row>
-    <row r="528" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A528" s="1" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C528" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D528" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E528" s="1" t="s">
         <v>13</v>
@@ -23084,13 +23087,13 @@
         <v>14</v>
       </c>
       <c r="G528" s="3">
-        <v>30000</v>
+        <v>90000</v>
       </c>
       <c r="H528" s="3">
-        <v>30000</v>
+        <v>90000</v>
       </c>
       <c r="I528" s="3">
-        <v>30000</v>
+        <v>90000</v>
       </c>
       <c r="J528" s="4" t="s">
         <v>125</v>
@@ -23100,21 +23103,21 @@
         <v>—</v>
       </c>
       <c r="L528" s="2">
-        <v>44676</v>
-      </c>
-    </row>
-    <row r="529" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44677</v>
+      </c>
+    </row>
+    <row r="529" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A529" s="1" t="s">
-        <v>46</v>
+        <v>505</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C529" s="1" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="D529" s="1" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E529" s="1" t="s">
         <v>13</v>
@@ -23123,13 +23126,13 @@
         <v>14</v>
       </c>
       <c r="G529" s="3">
-        <v>90000</v>
+        <v>35000</v>
       </c>
       <c r="H529" s="3">
-        <v>90000</v>
+        <v>35000</v>
       </c>
       <c r="I529" s="3">
-        <v>90000</v>
+        <v>35000</v>
       </c>
       <c r="J529" s="4" t="s">
         <v>125</v>
@@ -23142,7 +23145,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="530" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A530" s="1" t="s">
         <v>505</v>
       </c>
@@ -23153,7 +23156,7 @@
         <v>10</v>
       </c>
       <c r="D530" s="1" t="s">
-        <v>133</v>
+        <v>25</v>
       </c>
       <c r="E530" s="1" t="s">
         <v>13</v>
@@ -23181,33 +23184,33 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="531" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A531" s="1" t="s">
-        <v>505</v>
+        <v>46</v>
       </c>
       <c r="B531" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C531" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="D531" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E531" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F531" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G531" s="3">
-        <v>35000</v>
+        <v>60000</v>
       </c>
       <c r="H531" s="3">
-        <v>35000</v>
+        <v>60000</v>
       </c>
       <c r="I531" s="3">
-        <v>35000</v>
+        <v>60000</v>
       </c>
       <c r="J531" s="4" t="s">
         <v>125</v>
@@ -23217,7 +23220,7 @@
         <v>—</v>
       </c>
       <c r="L531" s="2">
-        <v>44677</v>
+        <v>44679</v>
       </c>
     </row>
     <row r="532" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23228,10 +23231,10 @@
         <v>5</v>
       </c>
       <c r="C532" s="1" t="s">
-        <v>46</v>
+        <v>189</v>
       </c>
       <c r="D532" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E532" s="1" t="s">
         <v>21</v>
@@ -23240,13 +23243,13 @@
         <v>14</v>
       </c>
       <c r="G532" s="3">
-        <v>60000</v>
+        <v>35000</v>
       </c>
       <c r="H532" s="3">
-        <v>60000</v>
+        <v>35000</v>
       </c>
       <c r="I532" s="3">
-        <v>60000</v>
+        <v>35000</v>
       </c>
       <c r="J532" s="4" t="s">
         <v>125</v>
@@ -23256,89 +23259,128 @@
         <v>—</v>
       </c>
       <c r="L532" s="2">
-        <v>44679</v>
+        <v>44684</v>
       </c>
     </row>
     <row r="533" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A533" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C533" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D533" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E533" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F533" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G533" s="3">
+        <v>30000</v>
+      </c>
+      <c r="H533" s="3">
+        <v>30000</v>
+      </c>
+      <c r="I533" s="3">
+        <v>0</v>
+      </c>
+      <c r="J533" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="K533" s="3">
+        <f>IF(Records[[#This Row],[Total]]-Records[[#This Row],[Credit]]=0,"—",Records[[#This Row],[Total]]-Records[[#This Row],[Credit]])</f>
+        <v>30000</v>
+      </c>
+      <c r="L533" s="2">
+        <v>44690</v>
+      </c>
+    </row>
+    <row r="534" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A534" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G533" s="3">
+      <c r="G534" s="3">
         <f>SUBTOTAL(109,Records[Total])</f>
-        <v>870000</v>
-      </c>
-      <c r="H533" s="3">
+        <v>65000</v>
+      </c>
+      <c r="H534" s="3">
         <f>SUBTOTAL(109,Records[Earnings])</f>
-        <v>850000</v>
-      </c>
-      <c r="I533" s="3">
+        <v>65000</v>
+      </c>
+      <c r="I534" s="3">
         <f>SUBTOTAL(109,Records[Credit])</f>
-        <v>842000</v>
-      </c>
-      <c r="J533" s="3"/>
-      <c r="K533" s="3">
+        <v>35000</v>
+      </c>
+      <c r="J534" s="3"/>
+      <c r="K534" s="3">
         <f>SUBTOTAL(109,Records[Balance])</f>
-        <v>28000</v>
-      </c>
-      <c r="L533" s="1">
+        <v>30000</v>
+      </c>
+      <c r="L534" s="1">
         <f>SUBTOTAL(103,Records[Date])</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="535" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G535" s="3"/>
-      <c r="K535" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="536" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G536" s="3"/>
+      <c r="K536" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="540" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H540" s="3"/>
+    <row r="541" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H541" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J455 J457:J1048576">
-    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="On Going">
+    <cfRule type="containsText" dxfId="29" priority="20" operator="containsText" text="On Going">
       <formula>NOT(ISERROR(SEARCH("On Going",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="28" priority="24" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K455 K457:K1048576">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="—">
+    <cfRule type="containsText" dxfId="27" priority="22" operator="containsText" text="—">
       <formula>NOT(ISERROR(SEARCH("—",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K455 K457:K460 K466:K517 K520:K532">
-    <cfRule type="notContainsText" dxfId="17" priority="21" operator="notContains" text="—">
+    <cfRule type="notContainsText" dxfId="26" priority="21" operator="notContains" text="—">
       <formula>ISERROR(SEARCH("—",K2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J456">
-    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",J456)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="On Going">
+    <cfRule type="containsText" dxfId="24" priority="10" operator="containsText" text="On Going">
       <formula>NOT(ISERROR(SEARCH("On Going",J456)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K456">
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="—">
+    <cfRule type="containsText" dxfId="22" priority="12" operator="containsText" text="—">
       <formula>NOT(ISERROR(SEARCH("—",K456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K456">
-    <cfRule type="notContainsText" dxfId="12" priority="11" operator="notContains" text="—">
+    <cfRule type="notContainsText" dxfId="21" priority="11" operator="notContains" text="—">
       <formula>ISERROR(SEARCH("—",K456))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K464">
-    <cfRule type="notContainsText" dxfId="11" priority="8" operator="notContains" text="—">
+    <cfRule type="notContainsText" dxfId="20" priority="8" operator="notContains" text="—">
       <formula>ISERROR(SEARCH("—",K464))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23352,11 +23394,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E90C186-FC8D-43AC-9355-F281FD1A44FE}">
-  <dimension ref="A1:I996"/>
+  <dimension ref="A1:I998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D982" sqref="D982"/>
+      <selection pane="bottomLeft" activeCell="D983" sqref="D983"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51891,89 +51933,89 @@
     </row>
     <row r="981" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A981" t="s">
+        <v>439</v>
+      </c>
+      <c r="B981" t="s">
+        <v>293</v>
+      </c>
+      <c r="C981" s="12">
+        <v>5000</v>
+      </c>
+      <c r="D981" s="12">
+        <v>5000</v>
+      </c>
+      <c r="E981" s="15" t="str">
+        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
+        <v>—</v>
+      </c>
+      <c r="F981" s="9" t="str">
+        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
+        <v>Paid</v>
+      </c>
+      <c r="G981" s="11">
+        <v>44684</v>
+      </c>
+      <c r="H981" t="s">
+        <v>538</v>
+      </c>
+      <c r="I981">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="982" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A982" t="s">
+        <v>497</v>
+      </c>
+      <c r="B982" t="s">
+        <v>293</v>
+      </c>
+      <c r="C982" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D982" s="12">
+        <v>2000</v>
+      </c>
+      <c r="E982" s="15" t="str">
+        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
+        <v>—</v>
+      </c>
+      <c r="F982" s="9" t="str">
+        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
+        <v>Paid</v>
+      </c>
+      <c r="G982" s="11">
+        <v>44684</v>
+      </c>
+      <c r="H982" t="s">
+        <v>538</v>
+      </c>
+      <c r="I982">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="983" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A983" t="s">
         <v>517</v>
       </c>
-      <c r="B981" t="s">
+      <c r="B983" t="s">
         <v>296</v>
       </c>
-      <c r="C981" s="12">
+      <c r="C983" s="12">
         <v>100000</v>
       </c>
-      <c r="D981" s="12">
+      <c r="D983" s="12">
         <v>0</v>
       </c>
-      <c r="E981" s="15">
+      <c r="E983" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
         <v>100000</v>
-      </c>
-      <c r="F981" s="9" t="str">
-        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
-        <v>Unpaid</v>
-      </c>
-      <c r="G981" s="11">
-        <v>44686</v>
-      </c>
-      <c r="H981" t="s">
-        <v>538</v>
-      </c>
-      <c r="I981">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="982" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A982" t="s">
-        <v>191</v>
-      </c>
-      <c r="B982" t="s">
-        <v>296</v>
-      </c>
-      <c r="C982" s="12">
-        <v>210000</v>
-      </c>
-      <c r="D982" s="12">
-        <v>0</v>
-      </c>
-      <c r="E982" s="15">
-        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>210000</v>
-      </c>
-      <c r="F982" s="9" t="str">
-        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
-        <v>Unpaid</v>
-      </c>
-      <c r="G982" s="11">
-        <v>44686</v>
-      </c>
-      <c r="H982" t="s">
-        <v>538</v>
-      </c>
-      <c r="I982">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="983" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A983" t="s">
-        <v>287</v>
-      </c>
-      <c r="B983" t="s">
-        <v>298</v>
-      </c>
-      <c r="C983" s="12">
-        <v>86000</v>
-      </c>
-      <c r="D983" s="12">
-        <v>0</v>
-      </c>
-      <c r="E983" s="15">
-        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>86000</v>
       </c>
       <c r="F983" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
         <v>Unpaid</v>
       </c>
       <c r="G983" s="11">
-        <v>44699</v>
+        <v>44686</v>
       </c>
       <c r="H983" t="s">
         <v>538</v>
@@ -51984,27 +52026,27 @@
     </row>
     <row r="984" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A984" t="s">
-        <v>551</v>
+        <v>191</v>
       </c>
       <c r="B984" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C984" s="12">
-        <v>70000</v>
+        <v>210000</v>
       </c>
       <c r="D984" s="12">
         <v>0</v>
       </c>
       <c r="E984" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>70000</v>
+        <v>210000</v>
       </c>
       <c r="F984" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
         <v>Unpaid</v>
       </c>
       <c r="G984" s="11">
-        <v>44699</v>
+        <v>44686</v>
       </c>
       <c r="H984" t="s">
         <v>538</v>
@@ -52015,20 +52057,20 @@
     </row>
     <row r="985" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A985" t="s">
-        <v>245</v>
+        <v>287</v>
       </c>
       <c r="B985" t="s">
         <v>298</v>
       </c>
       <c r="C985" s="12">
-        <v>50000</v>
+        <v>86000</v>
       </c>
       <c r="D985" s="12">
         <v>0</v>
       </c>
       <c r="E985" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>50000</v>
+        <v>86000</v>
       </c>
       <c r="F985" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52046,20 +52088,20 @@
     </row>
     <row r="986" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A986" t="s">
-        <v>146</v>
+        <v>551</v>
       </c>
       <c r="B986" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C986" s="12">
-        <v>26900</v>
+        <v>70000</v>
       </c>
       <c r="D986" s="12">
         <v>0</v>
       </c>
       <c r="E986" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>26900</v>
+        <v>70000</v>
       </c>
       <c r="F986" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52077,20 +52119,20 @@
     </row>
     <row r="987" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A987" t="s">
-        <v>159</v>
+        <v>245</v>
       </c>
       <c r="B987" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C987" s="12">
-        <v>69900</v>
+        <v>50000</v>
       </c>
       <c r="D987" s="12">
         <v>0</v>
       </c>
       <c r="E987" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>69900</v>
+        <v>50000</v>
       </c>
       <c r="F987" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52108,20 +52150,20 @@
     </row>
     <row r="988" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A988" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
       <c r="B988" t="s">
         <v>299</v>
       </c>
       <c r="C988" s="12">
-        <v>60000</v>
+        <v>26900</v>
       </c>
       <c r="D988" s="12">
         <v>0</v>
       </c>
       <c r="E988" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>60000</v>
+        <v>26900</v>
       </c>
       <c r="F988" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52139,20 +52181,20 @@
     </row>
     <row r="989" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A989" t="s">
-        <v>465</v>
+        <v>159</v>
       </c>
       <c r="B989" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C989" s="12">
-        <v>32000</v>
+        <v>69900</v>
       </c>
       <c r="D989" s="12">
         <v>0</v>
       </c>
       <c r="E989" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>32000</v>
+        <v>69900</v>
       </c>
       <c r="F989" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52170,20 +52212,20 @@
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A990" t="s">
-        <v>537</v>
+        <v>185</v>
       </c>
       <c r="B990" t="s">
         <v>299</v>
       </c>
       <c r="C990" s="12">
-        <v>9050</v>
+        <v>60000</v>
       </c>
       <c r="D990" s="12">
         <v>0</v>
       </c>
       <c r="E990" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>9050</v>
+        <v>60000</v>
       </c>
       <c r="F990" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52201,20 +52243,20 @@
     </row>
     <row r="991" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A991" t="s">
-        <v>536</v>
+        <v>465</v>
       </c>
       <c r="B991" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C991" s="12">
-        <v>18400</v>
+        <v>32000</v>
       </c>
       <c r="D991" s="12">
         <v>0</v>
       </c>
       <c r="E991" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>18400</v>
+        <v>32000</v>
       </c>
       <c r="F991" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52227,25 +52269,25 @@
         <v>538</v>
       </c>
       <c r="I991">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="992" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A992" t="s">
-        <v>432</v>
+        <v>537</v>
       </c>
       <c r="B992" t="s">
         <v>299</v>
       </c>
       <c r="C992" s="12">
-        <v>138500</v>
+        <v>9050</v>
       </c>
       <c r="D992" s="12">
         <v>0</v>
       </c>
       <c r="E992" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>138500</v>
+        <v>9050</v>
       </c>
       <c r="F992" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52263,20 +52305,20 @@
     </row>
     <row r="993" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A993" t="s">
-        <v>364</v>
+        <v>536</v>
       </c>
       <c r="B993" t="s">
         <v>299</v>
       </c>
       <c r="C993" s="12">
-        <v>70700</v>
+        <v>18400</v>
       </c>
       <c r="D993" s="12">
         <v>0</v>
       </c>
       <c r="E993" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>70700</v>
+        <v>18400</v>
       </c>
       <c r="F993" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52289,25 +52331,25 @@
         <v>538</v>
       </c>
       <c r="I993">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="994" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A994" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="B994" t="s">
         <v>299</v>
       </c>
       <c r="C994" s="12">
-        <v>66250</v>
+        <v>138500</v>
       </c>
       <c r="D994" s="12">
         <v>0</v>
       </c>
       <c r="E994" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>66250</v>
+        <v>138500</v>
       </c>
       <c r="F994" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52325,20 +52367,20 @@
     </row>
     <row r="995" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A995" t="s">
-        <v>415</v>
+        <v>364</v>
       </c>
       <c r="B995" t="s">
         <v>299</v>
       </c>
       <c r="C995" s="12">
-        <v>100000</v>
+        <v>70700</v>
       </c>
       <c r="D995" s="12">
         <v>0</v>
       </c>
       <c r="E995" s="15">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
-        <v>100000</v>
+        <v>70700</v>
       </c>
       <c r="F995" s="9" t="str">
         <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
@@ -52351,49 +52393,111 @@
         <v>538</v>
       </c>
       <c r="I995">
-        <v>20222</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="996" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A996" t="s">
+        <v>363</v>
+      </c>
+      <c r="B996" t="s">
+        <v>299</v>
+      </c>
+      <c r="C996" s="12">
+        <v>66250</v>
+      </c>
+      <c r="D996" s="12">
+        <v>0</v>
+      </c>
+      <c r="E996" s="15">
+        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
+        <v>66250</v>
+      </c>
+      <c r="F996" s="9" t="str">
+        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
+        <v>Unpaid</v>
+      </c>
+      <c r="G996" s="11">
+        <v>44699</v>
+      </c>
+      <c r="H996" t="s">
+        <v>538</v>
+      </c>
+      <c r="I996">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="997" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A997" t="s">
+        <v>415</v>
+      </c>
+      <c r="B997" t="s">
+        <v>299</v>
+      </c>
+      <c r="C997" s="12">
+        <v>100000</v>
+      </c>
+      <c r="D997" s="12">
+        <v>0</v>
+      </c>
+      <c r="E997" s="15">
+        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"—",Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]])</f>
+        <v>100000</v>
+      </c>
+      <c r="F997" s="9" t="str">
+        <f>IF(Tabla3[[#This Row],[Amount]]-Tabla3[[#This Row],[Credit]]=0,"Paid","Unpaid")</f>
+        <v>Unpaid</v>
+      </c>
+      <c r="G997" s="11">
+        <v>44699</v>
+      </c>
+      <c r="H997" t="s">
+        <v>538</v>
+      </c>
+      <c r="I997">
+        <v>20222</v>
+      </c>
+    </row>
+    <row r="998" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A998" t="s">
         <v>17</v>
       </c>
-      <c r="C996" s="14">
+      <c r="C998" s="14">
         <f>SUBTOTAL(109,Tabla3[Amount])</f>
-        <v>1111700</v>
-      </c>
-      <c r="D996" s="14">
+        <v>1118700</v>
+      </c>
+      <c r="D998" s="14">
         <f>SUBTOTAL(109,Tabla3[Credit])</f>
-        <v>4000</v>
-      </c>
-      <c r="E996" s="10">
+        <v>11000</v>
+      </c>
+      <c r="E998" s="10">
         <f>SUBTOTAL(109,Tabla3[Balance])</f>
         <v>1107700</v>
       </c>
-      <c r="G996"/>
+      <c r="G998"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="F927 E963:F995">
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="—">
+  <conditionalFormatting sqref="F927 E963:F997">
+    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="—">
       <formula>NOT(ISERROR(SEARCH("—",E927)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F995">
-    <cfRule type="beginsWith" dxfId="9" priority="7" operator="beginsWith" text="Unpaid">
+  <conditionalFormatting sqref="F2:F997">
+    <cfRule type="beginsWith" dxfId="18" priority="7" operator="beginsWith" text="Unpaid">
       <formula>LEFT(F2,LEN("Unpaid"))="Unpaid"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="Paid">
+    <cfRule type="beginsWith" dxfId="17" priority="8" operator="beginsWith" text="Paid">
       <formula>LEFT(F2,LEN("Paid"))="Paid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F928:F954 E910:E954 E955:F962">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="—">
+    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="—">
       <formula>NOT(ISERROR(SEARCH("—",E910)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F909 F910:F926">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="—">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="—">
       <formula>NOT(ISERROR(SEARCH("—",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52421,7 +52525,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F927 E963:F995</xm:sqref>
+          <xm:sqref>F927 E963:F997</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="6" operator="containsText" id="{BA095FE1-3F0C-466C-8201-7EB40AEDF688}">

</xml_diff>